<commit_message>
06-04-21: Order Being Placed. Please Finalize BOM
</commit_message>
<xml_diff>
--- a/SensorBoard/Project Outputs for SensorBoard/BOM/Bill of Materials-SensorBoard.xlsx
+++ b/SensorBoard/Project Outputs for SensorBoard/BOM/Bill of Materials-SensorBoard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\IoTAdvanced-Mesh+Gateway\SensorBoard\Project Outputs for SensorBoard\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\IoTAdvanced-Mesh-Gateway\SensorBoard\Project Outputs for SensorBoard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DD56914-65FC-4ACB-99FE-264C376B384C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F92975-47CF-443B-B6EF-DD2B669D5DBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7995" xr2:uid="{8EC7018F-CD37-4351-BE08-CAC7779E03FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0B122722-2BF6-439A-B7B5-F44C8CBB52F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-SensorBoard" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="168">
   <si>
     <t>DesignItemId</t>
   </si>
@@ -192,13 +192,13 @@
     <t>D9</t>
   </si>
   <si>
-    <t>ORH-R35A</t>
-  </si>
-  <si>
-    <t>RLED</t>
-  </si>
-  <si>
-    <t>OrangeRed 615~625nm 0805 Light Emitting Diodes (LED) RoHS</t>
+    <t>12-21SURC/S530-A3/TR8</t>
+  </si>
+  <si>
+    <t>RLED-RA</t>
+  </si>
+  <si>
+    <t>Red 624nm Right-Angle 1206 Light Emitting Diodes (LED) RoHS</t>
   </si>
   <si>
     <t>D10</t>
@@ -231,7 +231,13 @@
     <t>Pluggable Terminal Blocks SMT TB R/A HEADER 3.5MM, 4 POS</t>
   </si>
   <si>
-    <t>J2, J3, J11, J12</t>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>CONN_2213932-4_TEC-NoBody</t>
+  </si>
+  <si>
+    <t>J2, J3, J11, J12, J14</t>
   </si>
   <si>
     <t>CONN_2213932-4_TEC</t>
@@ -285,7 +291,7 @@
     <t>CUI PJ-102AH</t>
   </si>
   <si>
-    <t>Male Header 2x3</t>
+    <t>Female Header 2x3</t>
   </si>
   <si>
     <t>PEC03DAAN</t>
@@ -297,6 +303,21 @@
     <t>JP1</t>
   </si>
   <si>
+    <t>Female Header RA 2x3</t>
+  </si>
+  <si>
+    <t>Male Header 2x1</t>
+  </si>
+  <si>
+    <t>PEC02SAAN</t>
+  </si>
+  <si>
+    <t>Header, 100mil, 2x1, Tin, TH</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
     <t>ACM2012-121-2P-T002</t>
   </si>
   <si>
@@ -333,7 +354,7 @@
     <t>Resistor SMD 0805</t>
   </si>
   <si>
-    <t>R1</t>
+    <t>R1, R3, R4</t>
   </si>
   <si>
     <t>0R</t>
@@ -342,12 +363,6 @@
     <t>R2</t>
   </si>
   <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>R3, R4</t>
-  </si>
-  <si>
     <t>10ohm</t>
   </si>
   <si>
@@ -360,13 +375,13 @@
     <t>R7, R8, R11, R20</t>
   </si>
   <si>
-    <t>170ohm</t>
-  </si>
-  <si>
-    <t>R9, R10, R28</t>
-  </si>
-  <si>
-    <t>400k</t>
+    <t>33ohm</t>
+  </si>
+  <si>
+    <t>R9, R10</t>
+  </si>
+  <si>
+    <t>470k</t>
   </si>
   <si>
     <t>R12, R16, R21, R26</t>
@@ -375,7 +390,13 @@
     <t>100k</t>
   </si>
   <si>
-    <t>R13, R14, R15, R17, R19, R23, R24, R25</t>
+    <t>R13, R17, R19, R24</t>
+  </si>
+  <si>
+    <t>110k</t>
+  </si>
+  <si>
+    <t>R14, R15, R23, R25</t>
   </si>
   <si>
     <t>3.3k</t>
@@ -384,18 +405,24 @@
     <t>R18</t>
   </si>
   <si>
-    <t>1.62k</t>
+    <t>1.6k (1%)</t>
   </si>
   <si>
     <t>R22</t>
   </si>
   <si>
-    <t>290ohm</t>
+    <t>200ohm</t>
   </si>
   <si>
     <t>R27</t>
   </si>
   <si>
+    <t>130ohm</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
     <t>EVP-AWCD4A</t>
   </si>
   <si>
@@ -406,6 +433,21 @@
   </si>
   <si>
     <t>PANASONIC EVPAW</t>
+  </si>
+  <si>
+    <t>SNT-100-BK-G Jumper</t>
+  </si>
+  <si>
+    <t>SNT-100-BK-G</t>
+  </si>
+  <si>
+    <t>Shunt, 100mil, Gold plated, Black</t>
+  </si>
+  <si>
+    <t>SH-J1</t>
+  </si>
+  <si>
+    <t>Jumper</t>
   </si>
   <si>
     <t>TL3330AF260QG</t>
@@ -880,17 +922,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7DCA19-DA22-4683-AAE9-CB725C74C622}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20100A3-F8AB-4B37-A9AE-CB777A9629EE}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="7" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1282,96 +1326,96 @@
         <v>62</v>
       </c>
       <c r="G17" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G18" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="F19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="4">
+      <c r="D20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="4">
         <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G21" s="4">
         <v>1</v>
@@ -1379,45 +1423,45 @@
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="F22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="F23" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G23" s="4">
         <v>1</v>
@@ -1425,68 +1469,68 @@
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="F25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G26" s="4">
         <v>1</v>
@@ -1494,275 +1538,275 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G27" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G28" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G29" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G30" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G31" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="4">
         <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G32" s="4">
-        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G33" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G34" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G35" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="G36" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G37" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="C38" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="E38" s="3" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="G38" s="4">
         <v>1</v>
@@ -1770,145 +1814,237 @@
     </row>
     <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="F39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G39" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="F40" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G40" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="F41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G41" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="B42" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="B43" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G42" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="F43" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G43" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="E44" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="B45" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G44" s="4">
+      <c r="D45" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G48" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="31" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup scale="29" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
07-04-2021: Designs Complete. Order Placed
</commit_message>
<xml_diff>
--- a/SensorBoard/Project Outputs for SensorBoard/BOM/Bill of Materials-SensorBoard.xlsx
+++ b/SensorBoard/Project Outputs for SensorBoard/BOM/Bill of Materials-SensorBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\IoTAdvanced-Mesh-Gateway\SensorBoard\Project Outputs for SensorBoard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F92975-47CF-443B-B6EF-DD2B669D5DBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B05BD46-3DE7-418C-BB50-E0200B7F4DD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0B122722-2BF6-439A-B7B5-F44C8CBB52F8}"/>
+    <workbookView xWindow="7200" yWindow="3945" windowWidth="21600" windowHeight="11505" xr2:uid="{D06E21C2-789A-404E-A589-0488EF1CEEF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-SensorBoard" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="169">
   <si>
     <t>DesignItemId</t>
   </si>
@@ -75,7 +75,7 @@
     <t>0.1uF</t>
   </si>
   <si>
-    <t>C2, C4, C5, C6</t>
+    <t>C2, C4, C5</t>
   </si>
   <si>
     <t>1uF</t>
@@ -291,21 +291,18 @@
     <t>CUI PJ-102AH</t>
   </si>
   <si>
-    <t>Female Header 2x3</t>
+    <t>Male Header 2x3 RA</t>
   </si>
   <si>
     <t>PEC03DAAN</t>
   </si>
   <si>
-    <t>Header, 100mil, 3x2, Tin, TH</t>
+    <t>Header, Right Angle, 100mil, 3x2, Tin, TH</t>
   </si>
   <si>
     <t>JP1</t>
   </si>
   <si>
-    <t>Female Header RA 2x3</t>
-  </si>
-  <si>
     <t>Male Header 2x1</t>
   </si>
   <si>
@@ -423,16 +420,22 @@
     <t>R28</t>
   </si>
   <si>
-    <t>EVP-AWCD4A</t>
-  </si>
-  <si>
-    <t>3.0MM X 2.0MM / 2.4N / 0.13MM ST</t>
+    <t>120ohm</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>B3U-1000P</t>
+  </si>
+  <si>
+    <t>Tactile Switch SPST-NO Top Actuated Surface Mount</t>
   </si>
   <si>
     <t>S1</t>
   </si>
   <si>
-    <t>PANASONIC EVPAW</t>
+    <t>SW_B3U-1000P</t>
   </si>
   <si>
     <t>SNT-100-BK-G Jumper</t>
@@ -483,16 +486,16 @@
     <t>ESP32WROOM32UEM113EH6400UH3Q0</t>
   </si>
   <si>
-    <t>ISO3082DWR</t>
-  </si>
-  <si>
-    <t>ISO3082DWR RS-485 Transceiver</t>
-  </si>
-  <si>
-    <t>200-Kbps, half-duplex, 2.5-kVrms isolated RS-485 &amp; RS-422 transceiver 16-SOIC -40 to 85</t>
+    <t>MAX3485ESA+</t>
+  </si>
+  <si>
+    <t>1/1 Transceiver Half RS422, RS485 8-SOIC</t>
   </si>
   <si>
     <t>U2</t>
+  </si>
+  <si>
+    <t>SOIC127P600X175-8N</t>
   </si>
   <si>
     <t>SM712.TCT</t>
@@ -922,19 +925,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20100A3-F8AB-4B37-A9AE-CB777A9629EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E853FD-42AF-4415-85FE-360E23A57D09}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="7" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1004,7 +1005,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1458,7 +1459,7 @@
         <v>87</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>84</v>
@@ -1469,22 +1470,22 @@
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G24" s="4">
         <v>1</v>
@@ -1492,22 +1493,22 @@
     </row>
     <row r="25" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="F25" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G25" s="4">
         <v>1</v>
@@ -1515,22 +1516,22 @@
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="F26" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G26" s="4">
         <v>1</v>
@@ -1538,22 +1539,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G27" s="4">
         <v>3</v>
@@ -1561,22 +1562,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="E28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G28" s="4">
         <v>1</v>
@@ -1584,22 +1585,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G29" s="4">
         <v>2</v>
@@ -1607,22 +1608,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="E30" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G30" s="4">
         <v>4</v>
@@ -1630,22 +1631,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="E31" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G31" s="4">
         <v>2</v>
@@ -1653,22 +1654,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G32" s="4">
         <v>4</v>
@@ -1676,22 +1677,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="E33" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G33" s="4">
         <v>4</v>
@@ -1699,22 +1700,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G34" s="4">
         <v>4</v>
@@ -1722,22 +1723,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="E35" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G35" s="4">
         <v>1</v>
@@ -1745,22 +1746,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="E36" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G36" s="4">
         <v>1</v>
@@ -1768,22 +1769,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="E37" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G37" s="4">
         <v>1</v>
@@ -1791,68 +1792,68 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="G38" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="C39" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="E39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="B40" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G39" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="F40" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G40" s="4">
         <v>1</v>
@@ -1860,114 +1861,114 @@
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="F41" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="B42" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G41" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>141</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G42" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="E43" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="B44" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G43" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>148</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G44" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="F45" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G45" s="4">
         <v>1</v>
@@ -1975,76 +1976,99 @@
     </row>
     <row r="46" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="F46" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="B47" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G46" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="F47" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="B48" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G47" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="F48" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G48" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="B49" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G48" s="4">
+      <c r="E49" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G49" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="29" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup scale="30" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>